<commit_message>
Planning VMQ - bugs to fix
</commit_message>
<xml_diff>
--- a/spectoProject/configuration/handle_uploaded_file/Employees2.xlsx
+++ b/spectoProject/configuration/handle_uploaded_file/Employees2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F1555F-3FAB-4E2F-B47A-5E0974776236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17708BD9-CEE8-4CAA-BACC-318F21B3A25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="54">
   <si>
     <t>Mat</t>
   </si>
@@ -2015,6 +2015,9 @@
   </si>
   <si>
     <t>Responsable Fabrication</t>
+  </si>
+  <si>
+    <t>SELMI  Houssem</t>
   </si>
 </sst>
 </file>
@@ -2088,12 +2091,30 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -2164,7 +2185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2203,6 +2224,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2486,22 +2510,22 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.44140625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="14.88671875" customWidth="1"/>
     <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" customWidth="1"/>
@@ -2563,7 +2587,7 @@
       <c r="A2" s="6">
         <v>81780</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -2596,7 +2620,7 @@
       <c r="L2" s="8">
         <v>82151</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="15" t="s">
         <v>23</v>
       </c>
       <c r="N2" s="8">
@@ -2611,10 +2635,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>789432</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>42</v>
+        <v>21678</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>53</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>17</v>
@@ -2623,7 +2647,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -2644,10 +2668,10 @@
         <v>22</v>
       </c>
       <c r="L3" s="8">
-        <v>57676</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>46</v>
+        <v>82151</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="N3" s="8">
         <v>81813</v>
@@ -2661,10 +2685,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>13421</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>789432</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>42</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>17</v>
@@ -2694,10 +2718,10 @@
         <v>22</v>
       </c>
       <c r="L4" s="8">
-        <v>86594</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>47</v>
+        <v>57676</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="N4" s="8">
         <v>81813</v>
@@ -2711,10 +2735,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>33645</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>13421</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>17</v>
@@ -2746,7 +2770,7 @@
       <c r="L5" s="8">
         <v>86594</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="14" t="s">
         <v>47</v>
       </c>
       <c r="N5" s="8">
@@ -2761,10 +2785,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>82151</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
+        <v>33645</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>17</v>
@@ -2791,13 +2815,13 @@
         <v>21</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="L6" s="8">
-        <v>89723</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>48</v>
+        <v>86594</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="N6" s="8">
         <v>81813</v>
@@ -2811,10 +2835,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
-        <v>57676</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>82151</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>17</v>
@@ -2841,13 +2865,13 @@
         <v>21</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="L7" s="8">
-        <v>9909</v>
+        <v>89723</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" s="8">
         <v>81813</v>
@@ -2860,11 +2884,11 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>86594</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>47</v>
+      <c r="A8" s="6">
+        <v>57676</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>17</v>
@@ -2891,13 +2915,13 @@
         <v>21</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="L8" s="8">
-        <v>999594</v>
+        <v>9909</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N8" s="8">
         <v>81813</v>
@@ -2906,6 +2930,56 @@
         <v>24</v>
       </c>
       <c r="P8" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>86594</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="8">
+        <v>999594</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="8">
+        <v>81813</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2929,8 +3003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B3EF81-4203-42FC-A3E8-05E06B1944C3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C16"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>